<commit_message>
create load, price, interface flow data import functions
</commit_message>
<xml_diff>
--- a/Data/NPCC140/npcc.xlsx
+++ b/Data/NPCC140/npcc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EERL\NY-Simple-Net\NY-Simple-Net-main\Data\NPCC140\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBD2B21-E945-4D6C-AE05-3ED637BE93B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEE5AD0-94F9-4E43-BAED-D01A85123B33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="11" r:id="rId1"/>
@@ -1943,7 +1943,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1955,6 +1955,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1995,11 +2002,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5240,7 +5248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
@@ -17580,9 +17588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X234"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K185" sqref="K185"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F108" sqref="F108:F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20469,10 +20477,10 @@
       <c r="D45" t="s">
         <v>288</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="2">
         <v>43</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="2">
         <v>50</v>
       </c>
       <c r="G45">
@@ -20534,10 +20542,10 @@
       <c r="D46" t="s">
         <v>289</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="2">
         <v>43</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="2">
         <v>50</v>
       </c>
       <c r="G46">
@@ -23329,10 +23337,10 @@
       <c r="D89" t="s">
         <v>332</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="2">
         <v>73</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="2">
         <v>74</v>
       </c>
       <c r="G89">
@@ -23394,10 +23402,10 @@
       <c r="D90" t="s">
         <v>333</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="2">
         <v>73</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="2">
         <v>74</v>
       </c>
       <c r="G90">
@@ -23524,10 +23532,10 @@
       <c r="D92" t="s">
         <v>335</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="2">
         <v>74</v>
       </c>
-      <c r="F92">
+      <c r="F92" s="2">
         <v>78</v>
       </c>
       <c r="G92">
@@ -23589,10 +23597,10 @@
       <c r="D93" t="s">
         <v>336</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="2">
         <v>74</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="2">
         <v>78</v>
       </c>
       <c r="G93">
@@ -24304,10 +24312,10 @@
       <c r="D104" t="s">
         <v>347</v>
       </c>
-      <c r="E104">
+      <c r="E104" s="2">
         <v>85</v>
       </c>
-      <c r="F104">
+      <c r="F104" s="2">
         <v>88</v>
       </c>
       <c r="G104">
@@ -24369,10 +24377,10 @@
       <c r="D105" t="s">
         <v>348</v>
       </c>
-      <c r="E105">
+      <c r="E105" s="2">
         <v>85</v>
       </c>
-      <c r="F105">
+      <c r="F105" s="2">
         <v>88</v>
       </c>
       <c r="G105">
@@ -24434,10 +24442,10 @@
       <c r="D106" t="s">
         <v>349</v>
       </c>
-      <c r="E106">
+      <c r="E106" s="2">
         <v>85</v>
       </c>
-      <c r="F106">
+      <c r="F106" s="2">
         <v>105</v>
       </c>
       <c r="G106">
@@ -24499,10 +24507,10 @@
       <c r="D107" t="s">
         <v>350</v>
       </c>
-      <c r="E107">
+      <c r="E107" s="2">
         <v>85</v>
       </c>
-      <c r="F107">
+      <c r="F107" s="2">
         <v>105</v>
       </c>
       <c r="G107">
@@ -24564,10 +24572,10 @@
       <c r="D108" t="s">
         <v>351</v>
       </c>
-      <c r="E108">
+      <c r="E108" s="2">
         <v>85</v>
       </c>
-      <c r="F108">
+      <c r="F108" s="2">
         <v>112</v>
       </c>
       <c r="G108">
@@ -24629,10 +24637,10 @@
       <c r="D109" t="s">
         <v>352</v>
       </c>
-      <c r="E109">
+      <c r="E109" s="2">
         <v>85</v>
       </c>
-      <c r="F109">
+      <c r="F109" s="2">
         <v>112</v>
       </c>
       <c r="G109">
@@ -24824,10 +24832,10 @@
       <c r="D112" t="s">
         <v>355</v>
       </c>
-      <c r="E112">
+      <c r="E112" s="2">
         <v>88</v>
       </c>
-      <c r="F112">
+      <c r="F112" s="2">
         <v>105</v>
       </c>
       <c r="G112">
@@ -24889,10 +24897,10 @@
       <c r="D113" t="s">
         <v>356</v>
       </c>
-      <c r="E113">
+      <c r="E113" s="2">
         <v>88</v>
       </c>
-      <c r="F113">
+      <c r="F113" s="2">
         <v>105</v>
       </c>
       <c r="G113">
@@ -32809,6 +32817,7 @@
   </sheetData>
   <autoFilter ref="A1:X234" xr:uid="{8C945100-2036-4D5F-9A61-AFE09911C636}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>